<commit_message>
some change in framework, like adding util class and making UsersPage
</commit_message>
<xml_diff>
--- a/target/classes/Data.xlsx
+++ b/target/classes/Data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbhattacharjee\Desktop\CrossSkillingAutomation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A68FD2CC-387C-41D9-8C86-4E5E80F32586}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF1D53E-EE0B-47F3-B3AC-017BBF4FF454}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
   <si>
     <t>Name</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>tb_2</t>
+  </si>
+  <si>
+    <t>skills</t>
+  </si>
+  <si>
+    <t>React.js, Angular</t>
   </si>
 </sst>
 </file>
@@ -407,10 +413,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -423,9 +429,10 @@
     <col min="6" max="6" width="18" customWidth="1"/>
     <col min="7" max="7" width="17.88671875" customWidth="1"/>
     <col min="8" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -436,16 +443,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
       </c>
       <c r="H1" t="s">
         <v>7</v>
@@ -453,8 +460,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -464,17 +474,17 @@
       <c r="C2" t="s">
         <v>9</v>
       </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
         <v>23</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2">
-        <v>5</v>
       </c>
       <c r="H2" t="s">
         <v>13</v>
@@ -482,8 +492,11 @@
       <c r="I2" t="s">
         <v>8</v>
       </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -493,17 +506,17 @@
       <c r="C3" t="s">
         <v>14</v>
       </c>
-      <c r="D3">
+      <c r="D3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>6</v>
+      </c>
+      <c r="G3">
         <v>23</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3">
-        <v>6</v>
       </c>
       <c r="H3" t="s">
         <v>13</v>
@@ -511,8 +524,11 @@
       <c r="I3" t="s">
         <v>8</v>
       </c>
+      <c r="J3" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -522,23 +538,26 @@
       <c r="C4" t="s">
         <v>15</v>
       </c>
-      <c r="D4">
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>7</v>
+      </c>
+      <c r="G4">
         <v>23</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4">
-        <v>7</v>
       </c>
       <c r="H4" t="s">
         <v>13</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -548,5 +567,6 @@
     <hyperlink ref="B3:B4" r:id="rId2" display="tb@g.com" xr:uid="{7255DAAE-74E8-45BB-8358-5AD92D156021}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Resolved errors in Homepage Test
</commit_message>
<xml_diff>
--- a/target/classes/Data.xlsx
+++ b/target/classes/Data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbhattacharjee\Desktop\CrossSkillingAutomation\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF1D53E-EE0B-47F3-B3AC-017BBF4FF454}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08807A10-3165-4C7C-AF1D-AEA65317F47B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913" calcOnSave="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>Name</t>
   </si>
@@ -79,13 +80,22 @@
   </si>
   <si>
     <t>React.js, Angular</t>
+  </si>
+  <si>
+    <t>Admin Username</t>
+  </si>
+  <si>
+    <t>mentorAdmin</t>
+  </si>
+  <si>
+    <t>abc123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,6 +116,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFD69D85"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,9 +145,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -415,11 +434,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="13.5546875" customWidth="1"/>
     <col min="2" max="2" width="13.77734375" customWidth="1"/>
@@ -432,7 +451,7 @@
     <col min="10" max="10" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,7 +483,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -496,7 +515,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -528,7 +547,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -569,4 +588,40 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{764805B4-B67F-4815-90F1-AA9FA349C658}">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="17.88671875" customWidth="1"/>
+    <col min="2" max="2" width="12.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.6">
+      <c r="A2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>